<commit_message>
Added PSRAM numbers to calc
</commit_message>
<xml_diff>
--- a/Calculator.xlsx
+++ b/Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ninja\Documents\Github\RP2350-LCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345E0F2A-9FB3-4D94-8EB3-C07A0B375F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2DF9B5-083E-4310-A2FD-6DC84038EC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{61CDE1C2-C80F-44BF-B35A-D8347332F2DB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="46">
   <si>
     <t>LCD Specs</t>
   </si>
@@ -149,20 +149,33 @@
     <t>HSTX DDR/Lane</t>
   </si>
   <si>
-    <t>RAM-&gt;HSTX Rate(Full)</t>
-  </si>
-  <si>
     <t>Frame Buffer (Full)</t>
   </si>
   <si>
-    <t>RAM-&gt;HSTX Rate (565)</t>
-  </si>
-  <si>
     <t>RAM-&gt;HSTX Rate (DMA)</t>
   </si>
   <si>
+    <t>PSRAM Specs</t>
+  </si>
+  <si>
+    <t>Max Transfer Rate</t>
+  </si>
+  <si>
+    <t>Max Size</t>
+  </si>
+  <si>
+    <t>Mbit</t>
+  </si>
+  <si>
+    <t>Mem-&gt;HSTX Rate (565)</t>
+  </si>
+  <si>
+    <t>Mem-&gt;HSTX Rate(Full)</t>
+  </si>
+  <si>
     <t>Notes:
--DDR only works with 16 BPP (i.e. 565) as it uses the same 32 Bit buffer for 2 px</t>
+-DDR only works with 16 BPP (i.e. 565) as it uses the same 32 Bit buffer for 2 px
+-Actual PSRAM transfer rate will be slightly slower due to overhead, negligible for large read/writes, but high for random r/w</t>
   </si>
 </sst>
 </file>
@@ -170,7 +183,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -201,21 +214,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124E5A81-BFA8-457C-BD05-646535E66EE6}">
-  <dimension ref="B2:T33"/>
+  <dimension ref="B2:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,47 +578,55 @@
     <col min="10" max="10" width="13.33203125" customWidth="1"/>
     <col min="11" max="11" width="8.88671875" customWidth="1"/>
     <col min="12" max="12" width="6.6640625" customWidth="1"/>
-    <col min="14" max="14" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.88671875" customWidth="1"/>
     <col min="16" max="16" width="6.6640625" customWidth="1"/>
     <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.88671875" customWidth="1"/>
     <col min="20" max="20" width="6.6640625" customWidth="1"/>
+    <col min="22" max="22" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.88671875" customWidth="1"/>
+    <col min="24" max="24" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="J2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="N2" s="1" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="N2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="R2" s="1" t="s">
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="R2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="V2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1024</v>
+        <v>800</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -617,7 +636,7 @@
       </c>
       <c r="G3">
         <f>C6*C7</f>
-        <v>679540</v>
+        <v>404736</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -629,11 +648,11 @@
         <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O3">
         <f>(C3*C4*_xlfn.CEILING.MATH(C8,32))/(8*1024)</f>
-        <v>2400</v>
+        <v>1500</v>
       </c>
       <c r="P3" t="s">
         <v>21</v>
@@ -647,13 +666,23 @@
       <c r="T3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="V3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3">
+        <f>4*S3</f>
+        <v>600</v>
+      </c>
+      <c r="X3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4">
-        <v>600</v>
+        <v>480</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -663,7 +692,7 @@
       </c>
       <c r="G4">
         <f>G3*C5</f>
-        <v>40772400</v>
+        <v>24284160</v>
       </c>
       <c r="H4" t="s">
         <v>9</v>
@@ -682,7 +711,7 @@
       </c>
       <c r="O4">
         <f>(C3*C4*16)/(1024*8)</f>
-        <v>1200</v>
+        <v>750</v>
       </c>
       <c r="P4" t="s">
         <v>21</v>
@@ -696,8 +725,17 @@
       <c r="T4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="V4" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4">
+        <v>128</v>
+      </c>
+      <c r="X4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -710,9 +748,9 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <f>G4/1000000</f>
-        <v>40.772399999999998</v>
+        <v>24.28416</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -732,7 +770,7 @@
       </c>
       <c r="O5">
         <f>(C3*_xlfn.CEILING.MATH(C8,32))/(8*1024)</f>
-        <v>4</v>
+        <v>3.125</v>
       </c>
       <c r="P5" t="s">
         <v>21</v>
@@ -746,13 +784,23 @@
       <c r="T5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="V5" t="s">
+        <v>41</v>
+      </c>
+      <c r="W5">
+        <f>(W4/8)*1024</f>
+        <v>16384</v>
+      </c>
+      <c r="X5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>1114</v>
+        <v>816</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -760,9 +808,9 @@
       <c r="F6" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <f>G5*K4</f>
-        <v>856.22039999999993</v>
+        <v>509.96735999999999</v>
       </c>
       <c r="H6" t="s">
         <v>16</v>
@@ -772,7 +820,7 @@
       </c>
       <c r="O6">
         <f>(C3*16)/(8*1024)</f>
-        <v>2</v>
+        <v>1.5625</v>
       </c>
       <c r="P6" t="s">
         <v>21</v>
@@ -787,12 +835,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7">
-        <v>610</v>
+        <v>496</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -800,27 +848,27 @@
       <c r="F7" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <f>G5*K5</f>
-        <v>285.40679999999998</v>
+        <v>169.98912000000001</v>
       </c>
       <c r="H7" t="s">
         <v>16</v>
       </c>
       <c r="N7" t="s">
-        <v>37</v>
-      </c>
-      <c r="O7" s="7">
+        <v>44</v>
+      </c>
+      <c r="O7" s="2">
         <f>_xlfn.CEILING.MATH(C8,32)*G5</f>
-        <v>1304.7167999999999</v>
+        <v>777.09312</v>
       </c>
       <c r="P7" t="s">
         <v>16</v>
       </c>
       <c r="R7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S7" s="6">
+        <v>38</v>
+      </c>
+      <c r="S7">
         <f>32*S3</f>
         <v>4800</v>
       </c>
@@ -828,7 +876,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -841,31 +889,31 @@
       <c r="F8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <f>(1/(G4/C6))*1000000</f>
-        <v>27.3224043715847</v>
+        <v>33.602150537634408</v>
       </c>
       <c r="H8" t="s">
         <v>28</v>
       </c>
       <c r="N8" t="s">
-        <v>39</v>
-      </c>
-      <c r="O8" s="3">
+        <v>43</v>
+      </c>
+      <c r="O8" s="2">
         <f>16*G5</f>
-        <v>652.35839999999996</v>
+        <v>388.54656</v>
       </c>
       <c r="P8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>30</v>
       </c>
       <c r="C9">
         <f>C6-C3</f>
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -873,29 +921,29 @@
       <c r="F9" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <f>(S3*1000000)*(G8*0.0000001)</f>
-        <v>409.8360655737705</v>
+        <v>504.03225806451616</v>
       </c>
       <c r="H9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>31</v>
       </c>
       <c r="C10">
         <f>C7-C4</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
-        <v>41</v>
+      <c r="B18" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -980,16 +1028,21 @@
       <c r="T21" s="4"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="F25" s="1" t="s">
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="F25" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="J25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
@@ -1010,6 +1063,15 @@
       <c r="H26" t="s">
         <v>11</v>
       </c>
+      <c r="J26" t="s">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1024</v>
+      </c>
+      <c r="L26" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
@@ -1030,6 +1092,15 @@
       <c r="H27" t="s">
         <v>11</v>
       </c>
+      <c r="J27" t="s">
+        <v>2</v>
+      </c>
+      <c r="K27">
+        <v>600</v>
+      </c>
+      <c r="L27" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
@@ -1050,6 +1121,15 @@
       <c r="H28" t="s">
         <v>9</v>
       </c>
+      <c r="J28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28">
+        <v>60</v>
+      </c>
+      <c r="L28" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
@@ -1070,6 +1150,15 @@
       <c r="H29" t="s">
         <v>11</v>
       </c>
+      <c r="J29" t="s">
+        <v>5</v>
+      </c>
+      <c r="K29">
+        <v>1114</v>
+      </c>
+      <c r="L29" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
@@ -1090,6 +1179,15 @@
       <c r="H30" t="s">
         <v>11</v>
       </c>
+      <c r="J30" t="s">
+        <v>6</v>
+      </c>
+      <c r="K30">
+        <v>610</v>
+      </c>
+      <c r="L30" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
@@ -1110,6 +1208,15 @@
       <c r="H31" t="s">
         <v>13</v>
       </c>
+      <c r="J31" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31">
+        <v>18</v>
+      </c>
+      <c r="L31" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
@@ -1132,8 +1239,18 @@
       <c r="H32" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="J32" t="s">
+        <v>30</v>
+      </c>
+      <c r="K32">
+        <f>K29-K26</f>
+        <v>90</v>
+      </c>
+      <c r="L32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>31</v>
       </c>
@@ -1154,9 +1271,21 @@
       <c r="H33" t="s">
         <v>11</v>
       </c>
+      <c r="J33" t="s">
+        <v>31</v>
+      </c>
+      <c r="K33">
+        <f>K30-K27</f>
+        <v>10</v>
+      </c>
+      <c r="L33" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="J25:L25"/>
     <mergeCell ref="B18:T21"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="F25:H25"/>

</xml_diff>